<commit_message>
Only update dob constraint
</commit_message>
<xml_diff>
--- a/config/standard/forms/contact/person-create.xlsx
+++ b/config/standard/forms/contact/person-create.xlsx
@@ -935,7 +935,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -978,6 +978,11 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1134,7 +1139,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1251,6 +1256,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1291,7 +1300,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1303,7 +1312,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1410,11 +1419,11 @@
   <dimension ref="A1:AR87"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="N20" activeCellId="0" sqref="N20"/>
+      <selection pane="bottomRight" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1432,8 +1441,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="132.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="18.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="18.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="22.57"/>
@@ -2668,7 +2676,7 @@
       <c r="N20" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="O20" s="19" t="s">
+      <c r="O20" s="29" t="s">
         <v>102</v>
       </c>
       <c r="P20" s="13"/>
@@ -2738,7 +2746,7 @@
       <c r="O21" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="P21" s="29" t="s">
+      <c r="P21" s="30" t="s">
         <v>112</v>
       </c>
       <c r="Q21" s="14"/>
@@ -2809,7 +2817,7 @@
       <c r="O22" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="P22" s="29" t="s">
+      <c r="P22" s="30" t="s">
         <v>112</v>
       </c>
       <c r="Q22" s="14"/>
@@ -2908,10 +2916,10 @@
       <c r="AR23" s="12"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="31" t="s">
         <v>130</v>
       </c>
       <c r="C24" s="12" t="s">
@@ -2966,10 +2974,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="31" t="s">
         <v>142</v>
       </c>
       <c r="C25" s="25" t="s">
@@ -3009,7 +3017,7 @@
       <c r="V25" s="12"/>
       <c r="W25" s="25"/>
       <c r="X25" s="12"/>
-      <c r="Y25" s="31"/>
+      <c r="Y25" s="32"/>
       <c r="Z25" s="14"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="16"/>
@@ -3017,10 +3025,10 @@
       <c r="AD25" s="21"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="33" t="s">
         <v>150</v>
       </c>
       <c r="C26" s="25" t="s">
@@ -3063,10 +3071,10 @@
       <c r="AD26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="33" t="s">
         <v>157</v>
       </c>
       <c r="C27" s="25" t="s">
@@ -3595,7 +3603,7 @@
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="13"/>
-      <c r="E41" s="33"/>
+      <c r="E41" s="34"/>
       <c r="F41" s="20"/>
       <c r="G41" s="16"/>
       <c r="H41" s="17"/>
@@ -3612,7 +3620,7 @@
       <c r="U41" s="21"/>
       <c r="V41" s="12"/>
       <c r="Y41" s="13"/>
-      <c r="Z41" s="33"/>
+      <c r="Z41" s="34"/>
       <c r="AA41" s="20"/>
       <c r="AB41" s="16"/>
       <c r="AC41" s="17"/>
@@ -3846,7 +3854,7 @@
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
-      <c r="D50" s="34"/>
+      <c r="D50" s="35"/>
       <c r="E50" s="14"/>
       <c r="F50" s="20"/>
       <c r="G50" s="16"/>
@@ -3863,7 +3871,7 @@
       <c r="T50" s="17"/>
       <c r="U50" s="21"/>
       <c r="V50" s="12"/>
-      <c r="Y50" s="34"/>
+      <c r="Y50" s="35"/>
       <c r="Z50" s="14"/>
       <c r="AA50" s="20"/>
       <c r="AB50" s="16"/>
@@ -3874,7 +3882,7 @@
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
-      <c r="D51" s="34"/>
+      <c r="D51" s="35"/>
       <c r="E51" s="14"/>
       <c r="F51" s="20"/>
       <c r="G51" s="16"/>
@@ -3891,7 +3899,7 @@
       <c r="T51" s="17"/>
       <c r="U51" s="21"/>
       <c r="V51" s="12"/>
-      <c r="Y51" s="34"/>
+      <c r="Y51" s="35"/>
       <c r="Z51" s="14"/>
       <c r="AA51" s="20"/>
       <c r="AB51" s="16"/>
@@ -3902,7 +3910,7 @@
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
-      <c r="D52" s="34"/>
+      <c r="D52" s="35"/>
       <c r="E52" s="14"/>
       <c r="F52" s="20"/>
       <c r="G52" s="16"/>
@@ -3919,7 +3927,7 @@
       <c r="T52" s="17"/>
       <c r="U52" s="21"/>
       <c r="V52" s="12"/>
-      <c r="Y52" s="34"/>
+      <c r="Y52" s="35"/>
       <c r="Z52" s="14"/>
       <c r="AA52" s="20"/>
       <c r="AB52" s="16"/>
@@ -3930,7 +3938,7 @@
       <c r="A53" s="12"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
-      <c r="D53" s="34"/>
+      <c r="D53" s="35"/>
       <c r="E53" s="14"/>
       <c r="F53" s="20"/>
       <c r="G53" s="16"/>
@@ -3947,7 +3955,7 @@
       <c r="T53" s="17"/>
       <c r="U53" s="21"/>
       <c r="V53" s="12"/>
-      <c r="Y53" s="34"/>
+      <c r="Y53" s="35"/>
       <c r="Z53" s="14"/>
       <c r="AA53" s="20"/>
       <c r="AB53" s="16"/>
@@ -3958,7 +3966,7 @@
       <c r="A54" s="12"/>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
-      <c r="D54" s="34"/>
+      <c r="D54" s="35"/>
       <c r="E54" s="14"/>
       <c r="F54" s="20"/>
       <c r="G54" s="16"/>
@@ -3975,7 +3983,7 @@
       <c r="T54" s="17"/>
       <c r="U54" s="21"/>
       <c r="V54" s="12"/>
-      <c r="Y54" s="34"/>
+      <c r="Y54" s="35"/>
       <c r="Z54" s="14"/>
       <c r="AA54" s="20"/>
       <c r="AB54" s="16"/>
@@ -3986,8 +3994,8 @@
       <c r="A55" s="12"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="33"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="34"/>
       <c r="F55" s="20"/>
       <c r="G55" s="16"/>
       <c r="H55" s="17"/>
@@ -4003,8 +4011,8 @@
       <c r="T55" s="17"/>
       <c r="U55" s="21"/>
       <c r="V55" s="12"/>
-      <c r="Y55" s="34"/>
-      <c r="Z55" s="33"/>
+      <c r="Y55" s="35"/>
+      <c r="Z55" s="34"/>
       <c r="AA55" s="20"/>
       <c r="AB55" s="16"/>
       <c r="AC55" s="17"/>
@@ -4014,8 +4022,8 @@
       <c r="A56" s="12"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="33"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="34"/>
       <c r="F56" s="20"/>
       <c r="G56" s="16"/>
       <c r="H56" s="17"/>
@@ -4031,8 +4039,8 @@
       <c r="T56" s="17"/>
       <c r="U56" s="21"/>
       <c r="V56" s="12"/>
-      <c r="Y56" s="34"/>
-      <c r="Z56" s="33"/>
+      <c r="Y56" s="35"/>
+      <c r="Z56" s="34"/>
       <c r="AA56" s="20"/>
       <c r="AB56" s="16"/>
       <c r="AC56" s="17"/>
@@ -4042,7 +4050,7 @@
       <c r="A57" s="12"/>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
-      <c r="D57" s="34"/>
+      <c r="D57" s="35"/>
       <c r="E57" s="14"/>
       <c r="F57" s="20"/>
       <c r="G57" s="16"/>
@@ -4059,7 +4067,7 @@
       <c r="T57" s="17"/>
       <c r="U57" s="21"/>
       <c r="V57" s="12"/>
-      <c r="Y57" s="34"/>
+      <c r="Y57" s="35"/>
       <c r="Z57" s="14"/>
       <c r="AA57" s="20"/>
       <c r="AB57" s="16"/>
@@ -4351,7 +4359,7 @@
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
-      <c r="E68" s="33"/>
+      <c r="E68" s="34"/>
       <c r="F68" s="20"/>
       <c r="G68" s="16"/>
       <c r="H68" s="17"/>
@@ -4368,7 +4376,7 @@
       <c r="U68" s="21"/>
       <c r="V68" s="12"/>
       <c r="Y68" s="13"/>
-      <c r="Z68" s="33"/>
+      <c r="Z68" s="34"/>
       <c r="AA68" s="20"/>
       <c r="AB68" s="16"/>
       <c r="AC68" s="17"/>
@@ -4378,8 +4386,8 @@
       <c r="A69" s="12"/>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
-      <c r="D69" s="34"/>
-      <c r="E69" s="33"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="34"/>
       <c r="F69" s="20"/>
       <c r="G69" s="16"/>
       <c r="H69" s="17"/>
@@ -4395,8 +4403,8 @@
       <c r="T69" s="17"/>
       <c r="U69" s="21"/>
       <c r="V69" s="12"/>
-      <c r="Y69" s="34"/>
-      <c r="Z69" s="33"/>
+      <c r="Y69" s="35"/>
+      <c r="Z69" s="34"/>
       <c r="AA69" s="20"/>
       <c r="AB69" s="16"/>
       <c r="AC69" s="17"/>
@@ -5889,13 +5897,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -5935,22 +5943,22 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>173</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="39" t="s">
         <v>176</v>
       </c>
       <c r="G2" s="16" t="s">
@@ -5979,22 +5987,22 @@
       <c r="Z2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>180</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="39" t="s">
         <v>183</v>
       </c>
       <c r="G3" s="16" t="s">
@@ -6023,22 +6031,22 @@
       <c r="Z3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="40" t="s">
         <v>189</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="39" t="s">
         <v>191</v>
       </c>
       <c r="G4" s="16" t="s">
@@ -6067,22 +6075,22 @@
       <c r="Z4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="40" t="s">
         <v>196</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="39" t="s">
         <v>198</v>
       </c>
       <c r="G5" s="16" t="s">
@@ -6111,22 +6119,22 @@
       <c r="Z5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="40" t="s">
         <v>203</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="39" t="s">
         <v>205</v>
       </c>
       <c r="G6" s="16" t="s">
@@ -6155,22 +6163,22 @@
       <c r="Z6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="40" t="s">
         <v>209</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="39" t="s">
         <v>211</v>
       </c>
       <c r="G7" s="16" t="s">
@@ -6202,19 +6210,19 @@
       <c r="A8" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="40" t="s">
         <v>217</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="39" t="s">
         <v>98</v>
       </c>
       <c r="G8" s="16" t="s">
@@ -6246,13 +6254,13 @@
       <c r="A9" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="40" t="s">
         <v>224</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -6290,13 +6298,13 @@
       <c r="A10" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="41" t="s">
         <v>229</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="42" t="s">
         <v>230</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="40" t="s">
         <v>231</v>
       </c>
       <c r="E10" s="14" t="s">
@@ -6334,19 +6342,19 @@
       <c r="A11" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="41" t="s">
         <v>236</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="42" t="s">
         <v>237</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="40" t="s">
         <v>238</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="39" t="s">
         <v>240</v>
       </c>
       <c r="G11" s="16" t="s">
@@ -6378,22 +6386,22 @@
       <c r="A12" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="40" t="s">
         <v>244</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="43" t="s">
         <v>247</v>
       </c>
       <c r="H12" s="17"/>
@@ -6434,7 +6442,7 @@
       <c r="E13" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="39" t="s">
         <v>253</v>
       </c>
       <c r="G13" s="16" t="s">
@@ -6466,10 +6474,10 @@
       <c r="A14" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="42" t="s">
         <v>256</v>
       </c>
       <c r="D14" s="13" t="s">
@@ -6478,7 +6486,7 @@
       <c r="E14" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="39" t="s">
         <v>259</v>
       </c>
       <c r="G14" s="16" t="s">
@@ -6510,10 +6518,10 @@
       <c r="A15" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="41" t="s">
         <v>262</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="42" t="s">
         <v>263</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -6522,7 +6530,7 @@
       <c r="E15" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="39" t="s">
         <v>266</v>
       </c>
       <c r="G15" s="16" t="s">
@@ -6554,10 +6562,10 @@
       <c r="A16" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="41" t="s">
         <v>269</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="42" t="s">
         <v>270</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -6598,10 +6606,10 @@
       <c r="A17" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>276</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="42" t="s">
         <v>277</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -6610,7 +6618,7 @@
       <c r="E17" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="39" t="s">
         <v>280</v>
       </c>
       <c r="G17" s="16" t="s">
@@ -6735,9 +6743,9 @@
       <c r="B2" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="C2" s="43" t="str">
+      <c r="C2" s="44" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2018-12-10  12-35</v>
+        <v>2019-01-21  19-46</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12" t="s">

</xml_diff>